<commit_message>
implemented generating assignments with API
</commit_message>
<xml_diff>
--- a/Excel Generator/ExternalResources/Vorlage.xlsx
+++ b/Excel Generator/ExternalResources/Vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelTest\Documents\C#\Excel Generator\Excel Generator\ExternalResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E2E45-A511-446B-800D-46E9A39B71BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66C0A1-BE57-4149-B8F6-AC96FD88D9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1596" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabe" sheetId="1" r:id="rId1"/>
@@ -75,18 +75,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,18 +106,18 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="16"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -155,18 +147,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -179,32 +159,35 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -223,54 +206,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,44 +542,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="J1" s="17" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="J1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="J2" s="18">
+      <c r="J2" s="12">
         <v>0</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.2" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -607,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA7B2CE-F2F3-4AE6-96AD-AADEC09E7B0A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,42 +599,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="J1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="J1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="J2" s="16">
+      <c r="J2" s="17">
         <v>0</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.2" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -666,7 +645,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +674,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>1.5</v>
       </c>
     </row>
@@ -705,7 +684,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="14"/>
       <c r="B9">
         <v>1000</v>
       </c>
@@ -723,7 +702,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="15"/>
       <c r="B10">
         <v>100</v>
       </c>
@@ -746,12 +725,12 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added icon, improved template (is in german), fixed some bugs
</commit_message>
<xml_diff>
--- a/Excel Generator/ExternalResources/Vorlage.xlsx
+++ b/Excel Generator/ExternalResources/Vorlage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelTest\Documents\C#\Excel Generator\Excel Generator\ExternalResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\C SHARP\Excel Assignment Generator\Excel Generator\ExternalResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66C0A1-BE57-4149-B8F6-AC96FD88D9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512D3979-FE82-4160-9E2A-CCD17414D9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9165" yWindow="645" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabe" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Punkte:</t>
   </si>
@@ -69,13 +69,28 @@
   </si>
   <si>
     <t>Erreicht</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +134,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +212,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -205,11 +242,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -235,15 +296,57 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,50 +631,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="I1" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="J1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
       <c r="J2" s="12">
         <v>0</v>
       </c>
-      <c r="K2" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -585,50 +744,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA7B2CE-F2F3-4AE6-96AD-AADEC09E7B0A}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="I1" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="J1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="J2" s="17">
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="I2" s="10">
         <v>0</v>
       </c>
-      <c r="K2" s="10">
+      <c r="J2" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="27">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="28">
+        <f>A5+C5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="24">
+        <v>10</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="27">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="28">
+        <f>A7-C7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="24">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="27">
+        <v>4</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="29">
+        <f>A9*C9</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="26">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="25">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="29">
+        <f>A11*C11</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="24">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="25">
+        <v>5</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="30">
+        <f>A13/C13</f>
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -645,12 +894,12 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,33 +907,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9">
         <v>1000</v>
       </c>
@@ -701,8 +950,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10">
         <v>100</v>
       </c>
@@ -719,17 +968,17 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>

</xml_diff>